<commit_message>
Fixed: Some unexpected errors in UI
These error merged during demo of project
</commit_message>
<xml_diff>
--- a/proj1/marksheets/1401CB01.xlsx
+++ b/proj1/marksheets/1401CB01.xlsx
@@ -645,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>-2.5</v>
+        <v>-1</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>0</v>
@@ -662,12 +662,12 @@
         <v>70</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>-35</v>
+        <v>-14</v>
       </c>
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">
         <is>
-          <t>35.0/140</t>
+          <t>56/140</t>
         </is>
       </c>
     </row>

</xml_diff>